<commit_message>
Changed how mwtab format works and fixed tests and examples.
</commit_message>
<xml_diff>
--- a/examples/convert/mwtab/Saved Directives/mwtab_ms_conversion_directives.xlsx
+++ b/examples/convert/mwtab/Saved Directives/mwtab_ms_conversion_directives.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="126">
   <si>
     <t>#tags</t>
   </si>
@@ -91,12 +91,12 @@
     <t>Data</t>
   </si>
   <si>
+    <t>Extended</t>
+  </si>
+  <si>
     <t>Metabolites</t>
   </si>
   <si>
-    <t>Extended</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -250,7 +250,7 @@
     <t>*#.exclusion_headers</t>
   </si>
   <si>
-    <t>id,intensity,intensity%type,intensity%units,assignment,entity.id,protocol.id,formula,compound,isotopologue,isotopologue%type</t>
+    <t>id,intensity,intensity%type,intensity%units,assignment,assignment%method,entity.id,protocol.id,formula,compound,isotopologue,isotopologue%type</t>
   </si>
   <si>
     <t>intensity%type</t>
@@ -319,12 +319,12 @@
     <t>"Metabolite"=assignment,entity.id=intensity</t>
   </si>
   <si>
-    <t>"Metabolite"=assignment,"formula"=formula,"compound"=compound,"isotopologue"=isotopologue,"isotopologue%type"=isotopologue%type</t>
-  </si>
-  <si>
     <t>#.fields_to_headers</t>
   </si>
   <si>
+    <t>"Metabolite"=assignment</t>
+  </si>
+  <si>
     <t>#.table</t>
   </si>
   <si>
@@ -334,6 +334,12 @@
     <t>"Metabolite"=assignment,"sample_id"=entity.id</t>
   </si>
   <si>
+    <t>*#.optional_headers</t>
+  </si>
+  <si>
+    <t>assignment%method,formula,compound,isotopologue,isotopologue%type</t>
+  </si>
+  <si>
     <t>measurement</t>
   </si>
   <si>
@@ -379,13 +385,13 @@
     <t>matrix</t>
   </si>
   <si>
+    <t>#.values_to_str</t>
+  </si>
+  <si>
     <t>type=sample_prep</t>
   </si>
   <si>
     <t>type=treatment</t>
-  </si>
-  <si>
-    <t>#.values_to_str</t>
   </si>
 </sst>
 </file>
@@ -717,7 +723,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -765,7 +771,7 @@
         <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G4" t="s">
         <v>94</v>
@@ -785,7 +791,7 @@
         <v>104</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G5" t="s">
         <v>95</v>
@@ -805,7 +811,7 @@
         <v>104</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G6" t="s">
         <v>95</v>
@@ -825,7 +831,7 @@
         <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G7" t="s">
         <v>95</v>
@@ -845,7 +851,7 @@
         <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s">
         <v>95</v>
@@ -868,7 +874,7 @@
         <v>103</v>
       </c>
       <c r="F10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G10" t="s">
         <v>94</v>
@@ -888,7 +894,7 @@
         <v>104</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G11" t="s">
         <v>95</v>
@@ -908,7 +914,7 @@
         <v>104</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G12" t="s">
         <v>95</v>
@@ -928,7 +934,7 @@
         <v>104</v>
       </c>
       <c r="F13" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G13" t="s">
         <v>95</v>
@@ -948,7 +954,7 @@
         <v>104</v>
       </c>
       <c r="F14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G14" t="s">
         <v>95</v>
@@ -968,7 +974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -979,7 +985,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -990,7 +996,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1021,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1043,13 +1049,13 @@
         <v>103</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G24" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -1063,13 +1069,13 @@
         <v>104</v>
       </c>
       <c r="F25" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="B26" t="s">
         <v>19</v>
       </c>
@@ -1083,13 +1089,13 @@
         <v>104</v>
       </c>
       <c r="F26" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="B27" t="s">
         <v>20</v>
       </c>
@@ -1103,13 +1109,13 @@
         <v>104</v>
       </c>
       <c r="F27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G27" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="B28" t="s">
         <v>21</v>
       </c>
@@ -1123,13 +1129,13 @@
         <v>104</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -1143,13 +1149,13 @@
         <v>104</v>
       </c>
       <c r="F29" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G29" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1166,10 +1172,10 @@
         <v>96</v>
       </c>
       <c r="F31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G31" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H31" t="s">
         <v>103</v>
@@ -1177,8 +1183,11 @@
       <c r="I31" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -1195,211 +1204,221 @@
         <v>76</v>
       </c>
       <c r="G32" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H32" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" t="s">
+        <v>122</v>
+      </c>
+      <c r="J32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" t="s">
+        <v>117</v>
+      </c>
+      <c r="H34" t="s">
+        <v>119</v>
+      </c>
+      <c r="I34" t="s">
+        <v>103</v>
+      </c>
+      <c r="J34" t="s">
+        <v>94</v>
+      </c>
+      <c r="K34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" t="s">
+        <v>76</v>
+      </c>
+      <c r="H35" t="s">
+        <v>120</v>
+      </c>
+      <c r="I35" t="s">
+        <v>108</v>
+      </c>
+      <c r="J35" t="s">
+        <v>122</v>
+      </c>
+      <c r="K35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" t="s">
         <v>106</v>
       </c>
-      <c r="I32" t="s">
+      <c r="F37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" t="s">
+        <v>119</v>
+      </c>
+      <c r="I37" t="s">
+        <v>103</v>
+      </c>
+      <c r="J37" t="s">
+        <v>94</v>
+      </c>
+      <c r="K37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" t="s">
+        <v>76</v>
+      </c>
+      <c r="H38" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" t="s">
-        <v>98</v>
-      </c>
-      <c r="F33" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" t="s">
-        <v>118</v>
-      </c>
-      <c r="H33" t="s">
-        <v>106</v>
-      </c>
-      <c r="I33" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
+      <c r="I38" t="s">
+        <v>108</v>
+      </c>
+      <c r="J38" t="s">
+        <v>122</v>
+      </c>
+      <c r="K38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" t="s">
         <v>0</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B40" t="s">
         <v>23</v>
       </c>
-      <c r="C35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" t="s">
         <v>96</v>
       </c>
-      <c r="G35" t="s">
-        <v>115</v>
-      </c>
-      <c r="H35" t="s">
-        <v>117</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="E40" t="s">
         <v>103</v>
       </c>
-      <c r="J35" t="s">
+      <c r="F40" t="s">
         <v>94</v>
       </c>
-      <c r="K35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="B36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36" t="s">
-        <v>105</v>
-      </c>
-      <c r="F36" t="s">
-        <v>97</v>
-      </c>
-      <c r="G36" t="s">
-        <v>76</v>
-      </c>
-      <c r="H36" t="s">
-        <v>118</v>
-      </c>
-      <c r="I36" t="s">
-        <v>106</v>
-      </c>
-      <c r="J36" t="s">
-        <v>120</v>
-      </c>
-      <c r="K36" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" t="s">
+    </row>
+    <row r="41" spans="1:11">
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
         <v>0</v>
       </c>
-      <c r="B38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
         <v>57</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D43" t="s">
         <v>96</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E43" t="s">
         <v>103</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F43" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="B39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" t="s">
-        <v>106</v>
-      </c>
-      <c r="F39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" t="s">
-        <v>28</v>
-      </c>
-      <c r="C41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" t="s">
-        <v>96</v>
-      </c>
-      <c r="E41" t="s">
-        <v>103</v>
-      </c>
-      <c r="F41" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="B42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" t="s">
-        <v>80</v>
-      </c>
-      <c r="D42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E42" t="s">
-        <v>107</v>
-      </c>
-      <c r="F42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="B43" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" t="s">
-        <v>98</v>
-      </c>
-      <c r="E43" t="s">
-        <v>107</v>
-      </c>
-      <c r="F43" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="B44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D44" t="s">
         <v>98</v>
       </c>
       <c r="E44" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F44" t="s">
         <v>95</v>
@@ -1407,16 +1426,16 @@
     </row>
     <row r="45" spans="1:11">
       <c r="B45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D45" t="s">
         <v>98</v>
       </c>
       <c r="E45" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F45" t="s">
         <v>95</v>
@@ -1424,16 +1443,16 @@
     </row>
     <row r="46" spans="1:11">
       <c r="B46" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D46" t="s">
         <v>98</v>
       </c>
       <c r="E46" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F46" t="s">
         <v>95</v>
@@ -1441,16 +1460,16 @@
     </row>
     <row r="47" spans="1:11">
       <c r="B47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D47" t="s">
         <v>98</v>
       </c>
       <c r="E47" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F47" t="s">
         <v>95</v>
@@ -1458,16 +1477,16 @@
     </row>
     <row r="48" spans="1:11">
       <c r="B48" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C48" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D48" t="s">
         <v>98</v>
       </c>
       <c r="E48" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F48" t="s">
         <v>95</v>
@@ -1475,16 +1494,16 @@
     </row>
     <row r="49" spans="1:11">
       <c r="B49" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="D49" t="s">
         <v>98</v>
       </c>
       <c r="E49" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F49" t="s">
         <v>95</v>
@@ -1492,218 +1511,218 @@
     </row>
     <row r="50" spans="1:11">
       <c r="B50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="B51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" t="s">
+        <v>109</v>
+      </c>
+      <c r="F51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="B52" t="s">
         <v>37</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>87</v>
       </c>
-      <c r="D50" t="s">
-        <v>98</v>
-      </c>
-      <c r="E50" t="s">
-        <v>107</v>
-      </c>
-      <c r="F50" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" t="s">
+      <c r="D52" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52" t="s">
+        <v>109</v>
+      </c>
+      <c r="F52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" t="s">
         <v>0</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>38</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>88</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D54" t="s">
         <v>57</v>
       </c>
-      <c r="E52" t="s">
-        <v>108</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="E54" t="s">
+        <v>110</v>
+      </c>
+      <c r="F54" t="s">
         <v>96</v>
       </c>
-      <c r="G52" t="s">
-        <v>115</v>
-      </c>
-      <c r="H52" t="s">
+      <c r="G54" t="s">
         <v>117</v>
       </c>
-      <c r="I52" t="s">
+      <c r="H54" t="s">
+        <v>119</v>
+      </c>
+      <c r="I54" t="s">
         <v>103</v>
       </c>
-      <c r="J52" t="s">
-        <v>112</v>
-      </c>
-      <c r="K52" t="s">
+      <c r="J54" t="s">
+        <v>114</v>
+      </c>
+      <c r="K54" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="B53" t="s">
-        <v>39</v>
-      </c>
-      <c r="C53" t="s">
-        <v>89</v>
-      </c>
-      <c r="D53" t="s">
-        <v>62</v>
-      </c>
-      <c r="E53" t="s">
-        <v>98</v>
-      </c>
-      <c r="F53" t="s">
-        <v>97</v>
-      </c>
-      <c r="G53" t="s">
-        <v>119</v>
-      </c>
-      <c r="H53" t="s">
-        <v>118</v>
-      </c>
-      <c r="I53" t="s">
-        <v>104</v>
-      </c>
-      <c r="J53" t="s">
-        <v>121</v>
-      </c>
-      <c r="K53" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="B54" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" t="s">
-        <v>89</v>
-      </c>
-      <c r="D54" t="s">
-        <v>63</v>
-      </c>
-      <c r="E54" t="s">
-        <v>98</v>
-      </c>
-      <c r="F54" t="s">
-        <v>98</v>
-      </c>
-      <c r="G54" t="s">
-        <v>119</v>
-      </c>
-      <c r="H54" t="s">
-        <v>118</v>
-      </c>
-      <c r="I54" t="s">
-        <v>104</v>
-      </c>
-      <c r="J54" t="s">
-        <v>121</v>
-      </c>
-      <c r="K54" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="B55" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
         <v>89</v>
       </c>
       <c r="D55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E55" t="s">
         <v>98</v>
       </c>
       <c r="F55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G55" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H55" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I55" t="s">
         <v>104</v>
       </c>
       <c r="J55" t="s">
+        <v>124</v>
+      </c>
+      <c r="K55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="B56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" t="s">
+        <v>98</v>
+      </c>
+      <c r="F56" t="s">
+        <v>98</v>
+      </c>
+      <c r="G56" t="s">
         <v>121</v>
       </c>
-      <c r="K55" t="s">
+      <c r="H56" t="s">
+        <v>120</v>
+      </c>
+      <c r="I56" t="s">
+        <v>104</v>
+      </c>
+      <c r="J56" t="s">
+        <v>124</v>
+      </c>
+      <c r="K56" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" t="s">
+        <v>98</v>
+      </c>
+      <c r="G57" t="s">
+        <v>121</v>
+      </c>
+      <c r="H57" t="s">
+        <v>120</v>
+      </c>
+      <c r="I57" t="s">
+        <v>104</v>
+      </c>
+      <c r="J57" t="s">
+        <v>124</v>
+      </c>
+      <c r="K57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" t="s">
         <v>0</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>42</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>57</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D59" t="s">
         <v>96</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E59" t="s">
         <v>103</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F59" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="B58" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58" t="s">
-        <v>80</v>
-      </c>
-      <c r="D58" t="s">
-        <v>98</v>
-      </c>
-      <c r="E58" t="s">
-        <v>109</v>
-      </c>
-      <c r="F58" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="B59" t="s">
-        <v>30</v>
-      </c>
-      <c r="C59" t="s">
-        <v>81</v>
-      </c>
-      <c r="D59" t="s">
-        <v>98</v>
-      </c>
-      <c r="E59" t="s">
-        <v>109</v>
-      </c>
-      <c r="F59" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="B60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D60" t="s">
         <v>98</v>
       </c>
       <c r="E60" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F60" t="s">
         <v>95</v>
@@ -1711,16 +1730,16 @@
     </row>
     <row r="61" spans="1:11">
       <c r="B61" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C61" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D61" t="s">
         <v>98</v>
       </c>
       <c r="E61" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F61" t="s">
         <v>95</v>
@@ -1728,16 +1747,16 @@
     </row>
     <row r="62" spans="1:11">
       <c r="B62" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D62" t="s">
         <v>98</v>
       </c>
       <c r="E62" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F62" t="s">
         <v>95</v>
@@ -1745,16 +1764,16 @@
     </row>
     <row r="63" spans="1:11">
       <c r="B63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D63" t="s">
         <v>98</v>
       </c>
       <c r="E63" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F63" t="s">
         <v>95</v>
@@ -1762,16 +1781,16 @@
     </row>
     <row r="64" spans="1:11">
       <c r="B64" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D64" t="s">
         <v>98</v>
       </c>
       <c r="E64" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F64" t="s">
         <v>95</v>
@@ -1779,16 +1798,16 @@
     </row>
     <row r="65" spans="1:11">
       <c r="B65" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C65" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="D65" t="s">
         <v>98</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F65" t="s">
         <v>95</v>
@@ -1796,263 +1815,297 @@
     </row>
     <row r="66" spans="1:11">
       <c r="B66" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" t="s">
+        <v>86</v>
+      </c>
+      <c r="D66" t="s">
+        <v>98</v>
+      </c>
+      <c r="E66" t="s">
+        <v>111</v>
+      </c>
+      <c r="F66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="B67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C67" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" t="s">
+        <v>98</v>
+      </c>
+      <c r="E67" t="s">
+        <v>111</v>
+      </c>
+      <c r="F67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="B68" t="s">
         <v>44</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C68" t="s">
         <v>87</v>
       </c>
-      <c r="D66" t="s">
-        <v>98</v>
-      </c>
-      <c r="E66" t="s">
-        <v>109</v>
-      </c>
-      <c r="F66" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
-      <c r="A68" t="s">
+      <c r="D68" t="s">
+        <v>98</v>
+      </c>
+      <c r="E68" t="s">
+        <v>111</v>
+      </c>
+      <c r="F68" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" t="s">
         <v>0</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" t="s">
         <v>45</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C70" t="s">
         <v>57</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D70" t="s">
         <v>96</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E70" t="s">
         <v>103</v>
       </c>
-      <c r="F68" t="s">
-        <v>112</v>
-      </c>
-      <c r="G68" t="s">
+      <c r="F70" t="s">
+        <v>114</v>
+      </c>
+      <c r="G70" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
-      <c r="B69" t="s">
-        <v>46</v>
-      </c>
-      <c r="C69" t="s">
-        <v>90</v>
-      </c>
-      <c r="D69" t="s">
-        <v>98</v>
-      </c>
-      <c r="E69" t="s">
-        <v>110</v>
-      </c>
-      <c r="F69" t="s">
-        <v>116</v>
-      </c>
-      <c r="G69" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
-      <c r="B70" t="s">
-        <v>47</v>
-      </c>
-      <c r="C70" t="s">
-        <v>91</v>
-      </c>
-      <c r="D70" t="s">
-        <v>98</v>
-      </c>
-      <c r="E70" t="s">
-        <v>110</v>
-      </c>
-      <c r="F70" t="s">
-        <v>116</v>
-      </c>
-      <c r="G70" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:11">
       <c r="B71" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" t="s">
+        <v>90</v>
+      </c>
+      <c r="D71" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" t="s">
+        <v>112</v>
+      </c>
+      <c r="F71" t="s">
+        <v>118</v>
+      </c>
+      <c r="G71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="B72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" t="s">
+        <v>91</v>
+      </c>
+      <c r="D72" t="s">
+        <v>98</v>
+      </c>
+      <c r="E72" t="s">
+        <v>112</v>
+      </c>
+      <c r="F72" t="s">
+        <v>118</v>
+      </c>
+      <c r="G72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="B73" t="s">
         <v>48</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>92</v>
       </c>
-      <c r="D71" t="s">
-        <v>98</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="D73" t="s">
+        <v>98</v>
+      </c>
+      <c r="E73" t="s">
+        <v>112</v>
+      </c>
+      <c r="F73" t="s">
+        <v>118</v>
+      </c>
+      <c r="G73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" t="s">
+        <v>49</v>
+      </c>
+      <c r="C75" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" t="s">
+        <v>96</v>
+      </c>
+      <c r="E75" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="B76" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" t="s">
+        <v>93</v>
+      </c>
+      <c r="D76" t="s">
+        <v>98</v>
+      </c>
+      <c r="E76" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" t="s">
+        <v>88</v>
+      </c>
+      <c r="D78" t="s">
+        <v>57</v>
+      </c>
+      <c r="E78" t="s">
         <v>110</v>
       </c>
-      <c r="F71" t="s">
-        <v>116</v>
-      </c>
-      <c r="G71" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11">
-      <c r="A73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" t="s">
-        <v>49</v>
-      </c>
-      <c r="C73" t="s">
-        <v>69</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="F78" t="s">
         <v>96</v>
       </c>
-      <c r="E73" t="s">
+      <c r="G78" t="s">
+        <v>117</v>
+      </c>
+      <c r="H78" t="s">
+        <v>119</v>
+      </c>
+      <c r="I78" t="s">
+        <v>103</v>
+      </c>
+      <c r="J78" t="s">
+        <v>114</v>
+      </c>
+      <c r="K78" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11">
-      <c r="B74" t="s">
-        <v>50</v>
-      </c>
-      <c r="C74" t="s">
-        <v>93</v>
-      </c>
-      <c r="D74" t="s">
-        <v>98</v>
-      </c>
-      <c r="E74" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11">
-      <c r="A76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B76" t="s">
-        <v>51</v>
-      </c>
-      <c r="C76" t="s">
-        <v>88</v>
-      </c>
-      <c r="D76" t="s">
-        <v>57</v>
-      </c>
-      <c r="E76" t="s">
-        <v>108</v>
-      </c>
-      <c r="F76" t="s">
-        <v>96</v>
-      </c>
-      <c r="G76" t="s">
-        <v>115</v>
-      </c>
-      <c r="H76" t="s">
-        <v>117</v>
-      </c>
-      <c r="I76" t="s">
-        <v>103</v>
-      </c>
-      <c r="J76" t="s">
-        <v>112</v>
-      </c>
-      <c r="K76" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11">
-      <c r="B77" t="s">
-        <v>52</v>
-      </c>
-      <c r="C77" t="s">
-        <v>89</v>
-      </c>
-      <c r="D77" t="s">
-        <v>62</v>
-      </c>
-      <c r="E77" t="s">
-        <v>98</v>
-      </c>
-      <c r="F77" t="s">
-        <v>97</v>
-      </c>
-      <c r="G77" t="s">
-        <v>63</v>
-      </c>
-      <c r="H77" t="s">
-        <v>118</v>
-      </c>
-      <c r="I77" t="s">
-        <v>104</v>
-      </c>
-      <c r="J77" t="s">
-        <v>122</v>
-      </c>
-      <c r="K77" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11">
-      <c r="B78" t="s">
-        <v>53</v>
-      </c>
-      <c r="C78" t="s">
-        <v>89</v>
-      </c>
-      <c r="D78" t="s">
-        <v>63</v>
-      </c>
-      <c r="E78" t="s">
-        <v>98</v>
-      </c>
-      <c r="F78" t="s">
-        <v>98</v>
-      </c>
-      <c r="G78" t="s">
-        <v>63</v>
-      </c>
-      <c r="H78" t="s">
-        <v>118</v>
-      </c>
-      <c r="I78" t="s">
-        <v>104</v>
-      </c>
-      <c r="J78" t="s">
-        <v>122</v>
-      </c>
-      <c r="K78" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:11">
       <c r="B79" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C79" t="s">
         <v>89</v>
       </c>
       <c r="D79" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E79" t="s">
         <v>98</v>
       </c>
       <c r="F79" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G79" t="s">
         <v>63</v>
       </c>
       <c r="H79" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I79" t="s">
         <v>104</v>
       </c>
       <c r="J79" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K79" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="B80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C80" t="s">
+        <v>89</v>
+      </c>
+      <c r="D80" t="s">
+        <v>63</v>
+      </c>
+      <c r="E80" t="s">
+        <v>98</v>
+      </c>
+      <c r="F80" t="s">
+        <v>98</v>
+      </c>
+      <c r="G80" t="s">
+        <v>63</v>
+      </c>
+      <c r="H80" t="s">
+        <v>120</v>
+      </c>
+      <c r="I80" t="s">
+        <v>104</v>
+      </c>
+      <c r="J80" t="s">
+        <v>125</v>
+      </c>
+      <c r="K80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11">
+      <c r="B81" t="s">
+        <v>54</v>
+      </c>
+      <c r="C81" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" t="s">
+        <v>64</v>
+      </c>
+      <c r="E81" t="s">
+        <v>98</v>
+      </c>
+      <c r="F81" t="s">
+        <v>98</v>
+      </c>
+      <c r="G81" t="s">
+        <v>63</v>
+      </c>
+      <c r="H81" t="s">
+        <v>120</v>
+      </c>
+      <c r="I81" t="s">
+        <v>104</v>
+      </c>
+      <c r="J81" t="s">
+        <v>125</v>
+      </c>
+      <c r="K81" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>